<commit_message>
Day 1, in-class vision work.
</commit_message>
<xml_diff>
--- a/Labs/Lab06/golf ball values.xlsx
+++ b/Labs/Lab06/golf ball values.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\horvegc\Documents\Spring\ME435\Labs\Lab06\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27792" windowHeight="12588"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -95,6 +100,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -143,7 +151,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -178,7 +186,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,20 +398,20 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -426,7 +434,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -449,7 +457,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -472,7 +480,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -495,7 +503,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -518,7 +526,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -541,12 +549,12 @@
         <v>156</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -569,7 +577,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -592,7 +600,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -615,7 +623,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -638,7 +646,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -661,12 +669,12 @@
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>1</v>
       </c>
@@ -689,7 +697,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -712,7 +720,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -735,7 +743,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -758,7 +766,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -781,7 +789,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -817,7 +825,7 @@
       <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -831,7 +839,7 @@
       <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>